<commit_message>
update tally exception list
</commit_message>
<xml_diff>
--- a/downloads/tally/tally_ausnahmeliste.xlsx
+++ b/downloads/tally/tally_ausnahmeliste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\list\Documents\ocg-austria.github.io\downloads\tally\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\list\Documents\dev\tally\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4287EED4-AE07-4958-944D-2103058B3D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E240D625-9CC6-4233-B5F2-9A8CCD4F9C6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5790" yWindow="3270" windowWidth="23010" windowHeight="12210" xr2:uid="{3782226E-CEB5-4A7B-9145-17734ABF04E4}"/>
+    <workbookView xWindow="5415" yWindow="1770" windowWidth="23010" windowHeight="12210" xr2:uid="{3782226E-CEB5-4A7B-9145-17734ABF04E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,89 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <r>
-      <t xml:space="preserve">Ausnahmeliste für Tally
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">In dieser Liste können Werte eingetragen werden, welche von Tally ignoriert werden sollen. Hierfür stehen die folgenden zur Verfügung:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Debitorennummer allg. (Spalte C): </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Wird auf alle Zählungen angewandt
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Debitorennr Schulen (Spalte D):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Wird auf Zählungen von Schulen angewandt
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Debitorennr EB (Spalte E):</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Wird auf Zählungen von Erwachsenenbildung angewandt</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Debitorennr allg.</t>
   </si>
@@ -128,12 +46,138 @@
   <si>
     <t>Debitorennr EB</t>
   </si>
+  <si>
+    <t>Module</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ausnahmeliste für Tally</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">In dieser Liste können Werte eingetragen werden, welche von Tally ignoriert werden sollen. Hierfür stehen die folgenden zur Verfügung:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Debitorennummer allg. (Spalte B): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Wird auf alle Zählungen angewandt
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Debitorennr Schulen (Spalte C):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Wird auf Zählungen von Schulen angewandt
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Debitorennr EB (Spalte D):</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Wird auf Zählungen von Erwachsenenbildung angewandt</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Module (Spalte E): </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Alle Module, welche Text aus dieser Spalte enthalten werden ignoriert. (auf Groß- &amp; Kleinschreibung wird geachtet)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +216,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -187,7 +239,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -252,18 +304,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -607,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6117FD4-35F8-40B5-9DC3-2B8268A6523E}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,38 +691,49 @@
     <col min="2" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="F1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="4"/>
+    <row r="2" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6"/>
+      <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
+    <row r="3" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
+    <row r="5" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="5"/>
+    <row r="6" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:A6"/>
+    <mergeCell ref="A1:A8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>